<commit_message>
updated with recent series results and new prediction function
</commit_message>
<xml_diff>
--- a/output_csvs/predictions_2018.xlsx
+++ b/output_csvs/predictions_2018.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="21">
   <si>
     <t>Home</t>
   </si>
@@ -143,7 +143,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -152,14 +152,15 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -303,11 +304,11 @@
         </c:dLbls>
         <c:gapWidth val="20"/>
         <c:overlap val="-41"/>
-        <c:axId val="2053138864"/>
-        <c:axId val="2048316368"/>
+        <c:axId val="-803031888"/>
+        <c:axId val="-804486688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2053138864"/>
+        <c:axId val="-803031888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -347,7 +348,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2048316368"/>
+        <c:crossAx val="-804486688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -355,7 +356,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2048316368"/>
+        <c:axId val="-804486688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3.0"/>
@@ -405,7 +406,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2053138864"/>
+        <c:crossAx val="-803031888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="0.5"/>
@@ -1291,24 +1292,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="3" width="10.83203125" style="2"/>
-    <col min="4" max="4" width="19.6640625" style="5" customWidth="1"/>
-    <col min="5" max="7" width="10.83203125" style="1"/>
-    <col min="8" max="8" width="19.33203125" style="4" customWidth="1"/>
-    <col min="9" max="11" width="10.83203125" style="1"/>
-    <col min="12" max="12" width="20" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" style="4" customWidth="1"/>
+    <col min="5" max="7" width="10.83203125" style="2"/>
+    <col min="8" max="8" width="19.33203125" style="3" customWidth="1"/>
+    <col min="9" max="11" width="10.83203125" style="2"/>
+    <col min="12" max="12" width="20" style="2" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" style="2"/>
+    <col min="14" max="15" width="8.6640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="19.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -1318,10 +1322,10 @@
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -1333,7 +1337,7 @@
       <c r="H1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -1345,8 +1349,20 @@
       <c r="L1" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="M1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1356,10 +1372,10 @@
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>0.75634605929665799</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="2">
         <v>2</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -1368,10 +1384,10 @@
       <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="5">
         <v>0.57299999999999995</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2" s="2">
         <v>3</v>
       </c>
       <c r="J2" s="2" t="s">
@@ -1380,11 +1396,23 @@
       <c r="K2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="6">
+      <c r="L2" s="5">
         <v>0.61599999999999999</v>
       </c>
+      <c r="M2" s="2">
+        <v>4</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="5">
+        <v>0.66900000000000004</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1394,10 +1422,10 @@
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>0.65721639721073</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="2">
         <v>2</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -1406,10 +1434,10 @@
       <c r="G3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5">
         <v>0.497</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="2">
         <v>3</v>
       </c>
       <c r="J3" s="2" t="s">
@@ -1418,11 +1446,14 @@
       <c r="K3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="5">
         <v>0.66300000000000003</v>
       </c>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="5"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1432,10 +1463,10 @@
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>0.43457626826584</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="2">
         <v>2</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -1444,11 +1475,11 @@
       <c r="G4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <v>0.314</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -1458,10 +1489,10 @@
       <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>0.53905084588464003</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="2">
         <v>2</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -1470,11 +1501,11 @@
       <c r="G5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <v>0.47099999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -1484,11 +1515,11 @@
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>0.65444781051798095</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -1498,11 +1529,11 @@
       <c r="C7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>0.69483748991613503</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -1512,11 +1543,11 @@
       <c r="C8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>0.40319354516884598</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -1526,24 +1557,28 @@
       <c r="C9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>0.55847806176277304</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="6">
         <f>LN(0.76*0.66*0.43*0.46*0.65*0.69*0.4*0.56)/8</f>
         <v>-0.57605087175841685</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="6">
         <f>LN(0.43*0.5*0.31*0.47)/4</f>
         <v>-0.8658307041588631</v>
+      </c>
+      <c r="L12" s="2">
+        <f>LN(0.38*0.34)/2</f>
+        <v>-1.0231968438168177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>